<commit_message>
S04P12A401-115 [+] Edit DB 개요 마무리
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_total.xlsx
+++ b/DB/cocktailDB/cocktailDB_total.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\s04p12a401\DB\cocktailDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="article" sheetId="2" r:id="rId1"/>
@@ -17,10 +17,10 @@
     <sheet name="alcohol" sheetId="6" r:id="rId3"/>
     <sheet name="ingredient" sheetId="1" r:id="rId4"/>
     <sheet name="recipe" sheetId="3" r:id="rId5"/>
-    <sheet name="용어정리" sheetId="5" r:id="rId6"/>
+    <sheet name="cup" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">article!$C$1:$C$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">article!$C$1:$C$94</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="468">
   <si>
     <t>기저 주류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -740,21 +740,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이 칵테일의 이름은 마시고 난 뒤에 마치 사막에서 물을 찾는 듯한 느낌을 들게 해서 유래되었습니다. 맛도 이름처럼 매우 맵다고 합니다. 정확히는 플로팅을 사용하는 칵테일이지만 플로팅을 하지 않아도 맛은 변하지 않습니다.
-여담으로 바카디 151을 섞어 넣으면 'Hello on the Earth'라는 칵테일이 됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이름에 사워가 들어가지만 그렇게 신맛나는 칵테일은 아닙니다. 데킬라에 비해 들어가는 레몬 주스의 양이 적어 도수가 높으니 마실 때 주의하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>칵테일의 이름은 데킬라를 마시고 난 숙취를 의미합니다. 오렌지 주스와 그레나딘 시럽이 들어가 잘 넘어가기 때문에 주의해야 합니다. 본 칵테일과는 반대로 석양을 컨셉으로 한 데킬라 선셋이라는 칵테일도 존재합니다. 또한 데킬라를 제외시키면 선라이즈라는 이름의 논 알콜 칵테일이 됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데킬라 선라이즈가 태양이 뜨는 것을 모티브로 한 것과는 반대로 석양을 모티브로 한 칵테일입니다.
-그렇기 때문에 그레나딘 시럽이 위쪽에 부어지는 그라데이션을 볼 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -972,10 +962,6 @@
   </si>
   <si>
     <t>벨벳 해머</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>벨벳 해머ver2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1588,6 +1574,480 @@
   </si>
   <si>
     <t>한 잔 마시면 지진을 느낄 정도로 독한 칵테일입니다. 그에 걸맞게 47도라는 어마어마한 도수로 주의해야 합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">진에 라임 주스와 라임을 넣어 마시는 칵테일입니다. 재료가 워낙 간단한지라 만들기 쉽고 단순한 만큼 맛의 밸런스가 요구됩니다.  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피즈 스타일의 칵테일 중에서 가장 유명한 칵테일입니다. '피즈'란 미국의 유명한 바텐더인 제리 토마스가 정립한 스타일 칵테일 입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아틸러리(Artillery)라고도 불립니다. 진과 스윗 베르무트를 1:1 비율로 섞고 오렌지 비터를 추가한 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핑크 레이디와 유사한 칵테일 중 하나입니다. 달걀 흰자가 들어가는 것은 맛을 내기 위한 것이 아니라 유화제 역할을 하는 것으로 흔들 때 특유의 흰 거품이 이는 것이 특징입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레몬 즙과 설탕 시럽, 탄산수가 들어가 새콤달콤하면서도 시원한 맛을 내는 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마티니의 강한 맛이 약간 달콤한 맛으로 여성들에게 인기가 좋습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름의 의미는 '(기독교의) 장로교 신자'이고 특유의 시원한 솔잎향과 심플한 맛으로 마니아층이 존해합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>‘다이아몬드 피즈’ 라고도 불립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핑크 레이디라는 이름의 유래는 1912년 영국 런던에서 공연된 동명의 연극이 흥행하고 열린 파티에서 그 여주인공을 연기한 여배우에게 바쳐진 데에서 유래한 것이며, 이후 오늘날까지 전해 내려온 것이라고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앙고스투라 비터를 사용한 간단한 칵테일로 영국 선원들이 진에 비터를 쳐서 약효도 보고 맛도 좀 낫게 만들어서 먹던 것에서 왔다고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갓 짜낸 레몬 주스의 색깔 때문에 옅은 흰색 내지는 미황색을 띄게 되는데 여기서 칵테일의 이름이 유래되었다고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탄산음료를 섞은 진 베이스 칵테일로 오래도록 사랑받은 칵테일 입니다. 청량감 덕분에 여름 대표 칵테일로 자리잡게 되었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 칵테일은 콥스 리바이버 뿐만 아니라 '아이 오프너', '포그 커터'라는 이름의 칵테일은 19세기부터 있어 왔습니다. 이들의 용도는 숙취 해소를 위해 아침에 눈떠 마시는 칵테일들이었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미모사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mimosa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뱀부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bamboo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뱅쇼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vin Chaud</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상그리아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sangaree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아페롤 스프리츠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aperol spritz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오후의 죽음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Death in the afternoon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Casanova</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키르</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단순히 오렌지 주스와 섞기만 하면 만들 수 있는 간단한 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1889년 일본의 요코하마에서 만들어진 칵테일입니다. 매우 섬세한 향을 가지고 있는 이유로 레몬 필을 짜주면 '아모르' 라는 칵테일로 바뀌게 됩니다. 일본주와 비슷한 맛을 가지고 있으며 도수도 낮기 때문에 일본 음식과도 잘 어울린다고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>따뜻한 와인'이란 뜻으로 제조 과정중에 따뜻하게 데우기 때문에 와인의 알콜은 거의 증발하여 무알콜에 가깝습니다. 프랑스에서 유래되어 추운 겨울 몸을 따뜻하게 마시는 것이 보통이나, 여름에 차갑게 마시기도 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스페인과 포르투갈에서 유래되어 와인에 과일을 많이 넣고 주스를 섞어 숙성시킨 술입니다. 샹그리아를 끓여서 뱅쇼처럼 끓여 먹기도 하지만 주로 차게 숙성하여 먹기때문에 뱅쇼에 비해 알코올 농도가 높은 편입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1950년대 이탈리아에서 생겨났으며, 감귤향 리큐르인 아페롤과 일종의 스파클링 와인인 드라이 프로세코 와인, 그리고 탄산수를 일정 비율로 섞어 마시는 칵테일입니다. 이탈리아에 여행 다녀온 사람이라면 호텔이나 음식점에서 한번쯤은 접해볼 만큼 무척 유명하고 대중적인 식전주입니다. 더운 여름날에 마시기 좋은 칵테일이라고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈센트 반 고흐덕에 유명한 독주인 압생트와 샴페인을 재료로 합니다. 맛은 압생트의 산초, 그리고 향신료향과 샴페인의 청량감이 복합적으로 느껴지는 오묘한 맛입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원래는 부르고뉴의 화이트 와인과 그 지방의 특산품인 카시스를 이용해 만든 칵테일로, 그 곳을 방문하는 외부인을 환영하기 위해 만들어졌다고 합니다. 처음 이름은 블랑 카스(Blanc Cass)였지만 이후 그 당시 시장의 이름을 따 시장키르(Major Kir)라고 불리게 되었으며 이후 줄여서 키르(Kir)라고 불리게 되었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리큐르</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-52</t>
+  </si>
+  <si>
+    <t>옥보단</t>
+  </si>
+  <si>
+    <t>골든 캐딜락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Golden Cadillac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래스호퍼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grasshopper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그린 위도우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green Widow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깔루아 밀크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kahlua Milk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미도리 사워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Midori Sour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이올렛 피즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Violet fizz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버블껌 보이 샷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bubble Gum Boy Shot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베일리스 밀크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baileys milk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Velvet Hammer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브레인 해머릿지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brain Hamorrhage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스칼렛 오하라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scarlett o'hara</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬로 진 피즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sloe Gin fizz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아메리카노</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Americano</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에일리언 브레인 해머릿지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alien Brain Hemorrhage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔젤 팁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Angel's tip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예거밤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jägerbomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>준벅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>June Bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카카오 피즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cacao Fizz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀵퍽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quick Fuck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테네시 왈츠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tennessee Waltz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>푸스 카페 레인보우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pusse Cafe Rainbow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피치 크러시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peach Crush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핌즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pimm's</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sex and zen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">어원은 폭격기 이름인 B-52로 이름 그대로 슈터 계열의 강렬한 한 잔입니다. 해외에선 간단하게 BIFI라고 부릅니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유래는 1952년 미국의 프랭크 클라인이라는 바텐더가 한 커플의 부탁으로 직접 만들어 준 것이라고 탄생했습니다. 이때 프랭크 클라인이 일하고 있던 곳이 캘리포니아의 골드 컨트리(Gold Country of California)라 불리는 지역이였고, 여기서 이름이 유래된 것이라고 합니다. 맛은 갈리아노와 크렘 드 카카오가 들어가 전체적으로 부드럽고도 고급스러운 느낌을 주는 편입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>녹색 빛깔을 띠고 있다고 하여 이런 이름이 붙었습니다. 맛은 민트의 향과 맛이 강하며 민트 초콜릿 아이스크림 맛 또는 박하사탕과도 유사하다고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛은 오렌지 주스와 블루 큐라소가 섞여 절묘하고도 새콤달콤합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우유에 커피 리큐르인 깔루아를 섞어 달콤하고 부드러우며 도수는 맥주와 비슷한 정도입니다. 우유를 섞는 양에 따라 도수는 달라지는데 깔루아의 달콤한 커피향과 우유의 부드러운 맛이 곁들여져서 술에 익숙하지 않은 사람들이 좋아합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멜론 리큐르의 한 종류인 미도리를 사용해 만드는 유명한 칵테일입니다. 미도리 사와 또는 미도리 사워라고도 합니다. 달콤한 멜론맛인 미도리와 새콤한 레몬향이 어우러져서 상큼한 색깔과 맛을 연출하는 것이 특징입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본적인 레시피는 평범한 '진 피즈'와 같지만 크렘 드 바이올렛을 사용하여 독특한 보라색과 화려한 꽃향기가 특징인 달콤한 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛은 들어가는 재료가 모두 단 맛이 나는 리큐르가 들어가서 매우 달며 베일리스가 들어가 있어 약간의 크리미함도 느껴질 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>달콤하고 부드러우나 베일리스에 포함된 아이리쉬 위스키 특유의 쓴맛이 약간 있습니다. 부드러운 맛으로 부담 없이 넘길 수 있는 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Velvet Hammer - ver2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벨벳 해머 - ver2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몽키 브레인이라 불리기도 합니다. 이름의 뜻은 뇌출혈이며, 실제 칵테일의 모습도 마치 뇌에서 피가 흐르는 생김새입니다. 마셨을 때의 느낌이 마치 입안에 가래를 머금은 듯한 느낌이라  식감이 좋은 편은 아니라고 합니다. 하지만 맛은 나쁘지 않다. 그레나딘 시럽과 베일리스 등등 모두 달콤한 리큐르만 들어가기 때문에 무척 단 맛이 나는 편입니다. 단 것을 좋아하는 사람에게는 적합한 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>붉은 색의 우아한 느낌을 주는 칵테일로 소설과 영화로 유명한 바람과 함께 사라지다에서 주인공인 스칼렛 오하라가 마신 칵테일에 그 이름을 붙여 만들어진 것이라 합니다. 맛은 서던 컴포트의 복숭아 향과 크랜베리 주스 그리고 라임의 상큼함이 조화를 이룹니다. 버전이 두 가지로 나뉘는데 콜린스 글라스를 사용하는 롱 드링크 버전과 마티니 글라스를 사용하는 숏 드링크 버전이 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자두의 일종인 슬로베리를 넣어 숙성시킨 슬로 진을 이용한 칵테일입니다. 기본적인 레시피는 '진 피즈'에서 진을 슬로진으로 변경한 것입니다. 그래서 맛이 진 피즈에 새콤한 맛을 살짝 더한 느낌이라고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이탈리아에서 베르무트에 소다수를 혼합한 것을 미국인들이 좋아해서 이를 두고 미국을 이미지화해서 이름을 붙인 것입니다. 주로 식전주로 쓰인다고 합니다. 원래는 비터 베르무트라는 쓴 맛이 나는 베르무트를 사용하지만 이후 캄파리를 사용하는 것으로 레시피가 바뀌었습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이름의 뜻은 외계인의 뇌출혈이다. 브레인 해머릿지에서 블루 큐라소만 추가된 버전입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">카카오 리큐르에 동량의 식물성 크림을 얇게 올려 만드는 칵테일입니다. 장식용 체리를 글라스에 살짝 담궜다 빼내면 크림의 층이 움직이면서 입술 모양과 비슷한 모양을 남긴다고 하여 '엔젤 키스'라는 별칭이 있습니다. 물론 엔젤 키스라는 칵테일은 따로 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리큐르인 예거마이스터와 에너지 드링크인 레드불을 섞어서 만드는 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔 가장자리에 설탕을 묻혀두는데 잔 가장자리에 묻은 설탕을 핥아먹는 모습 때문에 야한 칵테일로 통합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6월의 벌레라는 이름의 칵테일이지만 벌레보다는 6월의 푸르름을 표현한 칵테일입니다. 6월에 자주 등장하는 초록꽃무지에서 유래됐다는 이야기도 있습니다. 향과 맛이 달콤하기로 유명한 리큐르인 말리부가 들어가서 달달한 맛을 냅니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카카오를 넣어 숙성시켜 맛과 향을 첨가한 크렘 드 카카오을 이용한 칵테일입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도수가 높지만 맛은 달콤해서 비교적 빠르게 마시게 되는 칵테일인데 마시는 당신을 빠르게 침대로 보내서 본 작업에 들어가게 해 버린다는 의미의 위트 있는 작명이라는 평가가 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1949년, 이후 일본 바텐더 협회장이 된 하세가와 유키야스가 '술과 음악'이라는 잡지에 투고하여 유명해진 칵테일입니다. 국내에서는 잘 취급도지 않는 칵테일 입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">레인보우' 라는 이름으로 불리지만 정확한 이름은 '푸스 카페 레인보우'이며, 이름 그대로 7가지의 술이 들어가고 전부 섞이지 않게 올려야 하는 고난이도의 칵테일입니다. 샷 글라스를 이용해서 한번에 다 마십니다. 7개의 술을 사용하고 색을 더 구분하기 위해 원액에 가까운 상태로 만들어서 맛은 난잡해서 추천하지는 않습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복숭아 향이 살짝 나며 맛은 약간 새콤한 맛입니다. 도수가 매우 낮아서 여성들에게 인기가 많은 칵테일입니다. 가끔 진짜 복숭아를 으깨서 넣는 경우도 있다고 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영국의 술이자 리큐르 베이스인 동명의 칵테일의 명칭입니다. 영국에서 여름철에 굉장히 많이 소비되는 칵테일로 특히 야외활동을 할 때 자주 마신다고 합니다. 펀치류에 해당하는 칵테일의 특성상 재료를 크게 따지지 않아서 재료가 추가되거나 제외되기도 하지만 오이와 과일, 민트는 반드시 포함됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맥주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 칵테일의 이름은 마시고 난 뒤에 마치 사막에서 물을 찾는 듯한 느낌을 들게 해서 유래되었습니다. 맛도 이름처럼 매우 맵다고 합니다. 정확히는 플로팅을 사용하는 칵테일이지만 플로팅을 하지 않아도 맛은 변하지 않습니다. 여담으로 바카디 151을 섞어 넣으면 'Hello on the Earth'라는 칵테일이 됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 선라이즈가 태양이 뜨는 것을 모티브로 한 것과는 반대로 석양을 모티브로 한 칵테일입니다. 그렇기 때문에 그레나딘 시럽이 위쪽에 부어지는 그라데이션을 볼 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넣어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>섞어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>따라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마셔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cocktail_pk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1657,7 +2117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1733,13 +2193,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1787,10 +2256,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2071,28 +2543,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="6"/>
-    <col min="3" max="3" width="27.59765625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="8.796875" style="6"/>
+    <col min="3" max="3" width="27.59765625" style="7" customWidth="1"/>
     <col min="4" max="4" width="20.3984375" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" customWidth="1"/>
+    <col min="5" max="5" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2109,965 +2581,923 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="17"/>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="17"/>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="17"/>
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="17"/>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="17"/>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="17"/>
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="17"/>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="17"/>
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="17"/>
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="17"/>
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="17"/>
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="17"/>
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="17"/>
+      <c r="B15" s="6">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="17"/>
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="17"/>
+      <c r="B17" s="6">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="F17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
+      <c r="A18" s="17"/>
       <c r="B18" s="6">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="F18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="6">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="6">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="F20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="6">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="F21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="6">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="F22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="6">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="6">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="F24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="6">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F25" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="6">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="6">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="6">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29"/>
+      <c r="A29" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="B29" s="6">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>142</v>
+        <v>103</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="F29" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30"/>
       <c r="B30" s="6">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="F30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31"/>
       <c r="B31" s="6">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32"/>
       <c r="B32" s="6">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="F32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A33"/>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="6">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A34"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="6">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="F34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A35"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" s="6">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>289</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A36"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" s="6">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
-        <v>92</v>
+      <c r="C36" s="13" t="s">
+        <v>288</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A37"/>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" s="6">
         <v>36</v>
       </c>
-      <c r="C37" t="s">
-        <v>93</v>
+      <c r="C37" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="F37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A38"/>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B38" s="6">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="F38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A39"/>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" s="6">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A40"/>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" s="6">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="F40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A41"/>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" s="6">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>154</v>
+        <v>115</v>
+      </c>
+      <c r="E41" t="s">
+        <v>166</v>
       </c>
       <c r="F41" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A42"/>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" s="6">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>155</v>
+        <v>116</v>
+      </c>
+      <c r="E42" t="s">
+        <v>167</v>
       </c>
       <c r="F42" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A43"/>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" s="6">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>155</v>
+        <v>117</v>
+      </c>
+      <c r="E43" t="s">
+        <v>168</v>
       </c>
       <c r="F43" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A44"/>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" s="6">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>156</v>
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>169</v>
       </c>
       <c r="F44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>102</v>
-      </c>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B45" s="6">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>157</v>
+        <v>171</v>
+      </c>
+      <c r="E45" t="s">
+        <v>170</v>
       </c>
       <c r="F45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="6">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>158</v>
+        <v>120</v>
+      </c>
+      <c r="E46" t="s">
+        <v>172</v>
       </c>
       <c r="F46" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" s="6">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>159</v>
+        <v>121</v>
+      </c>
+      <c r="E47" t="s">
+        <v>173</v>
       </c>
       <c r="F47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="6">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>161</v>
+        <v>122</v>
+      </c>
+      <c r="E48" t="s">
+        <v>174</v>
       </c>
       <c r="F48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B49" s="6">
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>162</v>
+        <v>123</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="F49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B50" s="6">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>162</v>
+        <v>124</v>
+      </c>
+      <c r="E50" t="s">
+        <v>176</v>
       </c>
       <c r="F50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B51" s="6">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>292</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>162</v>
+        <v>125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>177</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B52" s="6">
         <v>51</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>163</v>
+      <c r="C52" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>178</v>
       </c>
       <c r="F52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B53" s="6">
         <v>52</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>164</v>
+      <c r="C53" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" t="s">
+        <v>179</v>
       </c>
       <c r="F53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B54" s="6">
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="E54" t="s">
+        <v>180</v>
       </c>
       <c r="F54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B55" s="6">
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>166</v>
+        <v>129</v>
+      </c>
+      <c r="E55" t="s">
+        <v>181</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A56" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="B56" s="6">
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>167</v>
+        <v>183</v>
+      </c>
+      <c r="E56" t="s">
+        <v>202</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B57" s="6">
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>184</v>
       </c>
       <c r="E57" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B58" s="6">
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>185</v>
       </c>
       <c r="E58" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B59" s="6">
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>186</v>
+      </c>
+      <c r="D59" t="s">
+        <v>404</v>
       </c>
       <c r="E59" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B60" s="6">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>444</v>
+      </c>
+      <c r="D60" t="s">
+        <v>443</v>
       </c>
       <c r="E60" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B61" s="6">
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E61" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="F61" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B62" s="6">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B63" s="6">
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B64" s="6">
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="E64" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -3078,10 +3508,10 @@
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>177</v>
+        <v>191</v>
+      </c>
+      <c r="E65" t="s">
+        <v>210</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3092,10 +3522,10 @@
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
       <c r="E66" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="F66" t="s">
         <v>55</v>
@@ -3106,10 +3536,10 @@
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="F67" t="s">
         <v>55</v>
@@ -3120,10 +3550,10 @@
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="E68" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="F68" t="s">
         <v>55</v>
@@ -3134,24 +3564,27 @@
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="E69" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="F69" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A70" s="6" t="s">
+        <v>196</v>
+      </c>
       <c r="B70" s="6">
         <v>69</v>
       </c>
-      <c r="C70" t="s">
-        <v>128</v>
+      <c r="C70" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="E70" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="F70" t="s">
         <v>55</v>
@@ -3161,28 +3594,25 @@
       <c r="B71" s="6">
         <v>70</v>
       </c>
-      <c r="C71" t="s">
-        <v>129</v>
+      <c r="C71" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="E71" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="F71" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A72" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="B72" s="6">
         <v>71</v>
       </c>
-      <c r="C72" t="s">
-        <v>185</v>
+      <c r="C72" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="E72" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="F72" t="s">
         <v>55</v>
@@ -3192,11 +3622,11 @@
       <c r="B73" s="6">
         <v>72</v>
       </c>
-      <c r="C73" t="s">
-        <v>186</v>
+      <c r="C73" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="E73" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="F73" t="s">
         <v>55</v>
@@ -3206,25 +3636,28 @@
       <c r="B74" s="6">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
-        <v>187</v>
+      <c r="C74" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="E74" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="F74" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A75" s="6" t="s">
+        <v>227</v>
+      </c>
       <c r="B75" s="6">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
-        <v>188</v>
-      </c>
-      <c r="E75" t="s">
-        <v>208</v>
+      <c r="C75" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="F75" t="s">
         <v>55</v>
@@ -3234,11 +3667,11 @@
       <c r="B76" s="6">
         <v>75</v>
       </c>
-      <c r="C76" t="s">
-        <v>189</v>
+      <c r="C76" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="E76" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
       <c r="F76" t="s">
         <v>55</v>
@@ -3248,11 +3681,11 @@
       <c r="B77" s="6">
         <v>76</v>
       </c>
-      <c r="C77" t="s">
-        <v>190</v>
+      <c r="C77" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="E77" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="F77" t="s">
         <v>55</v>
@@ -3262,11 +3695,11 @@
       <c r="B78" s="6">
         <v>77</v>
       </c>
-      <c r="C78" t="s">
-        <v>191</v>
+      <c r="C78" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="E78" t="s">
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="F78" t="s">
         <v>55</v>
@@ -3276,11 +3709,11 @@
       <c r="B79" s="6">
         <v>78</v>
       </c>
-      <c r="C79" t="s">
-        <v>192</v>
+      <c r="C79" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="E79" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
       <c r="F79" t="s">
         <v>55</v>
@@ -3290,11 +3723,11 @@
       <c r="B80" s="6">
         <v>79</v>
       </c>
-      <c r="C80" t="s">
-        <v>193</v>
+      <c r="C80" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="E80" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
       <c r="F80" t="s">
         <v>55</v>
@@ -3304,11 +3737,11 @@
       <c r="B81" s="6">
         <v>80</v>
       </c>
-      <c r="C81" t="s">
-        <v>194</v>
+      <c r="C81" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="E81" t="s">
-        <v>213</v>
+        <v>253</v>
       </c>
       <c r="F81" t="s">
         <v>55</v>
@@ -3318,11 +3751,11 @@
       <c r="B82" s="6">
         <v>81</v>
       </c>
-      <c r="C82" t="s">
-        <v>198</v>
+      <c r="C82" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="E82" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="F82" t="s">
         <v>55</v>
@@ -3332,11 +3765,11 @@
       <c r="B83" s="6">
         <v>82</v>
       </c>
-      <c r="C83" t="s">
-        <v>195</v>
+      <c r="C83" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="E83" t="s">
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="F83" t="s">
         <v>55</v>
@@ -3346,11 +3779,11 @@
       <c r="B84" s="6">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
-        <v>196</v>
+      <c r="C84" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="E84" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="F84" t="s">
         <v>55</v>
@@ -3360,28 +3793,25 @@
       <c r="B85" s="6">
         <v>84</v>
       </c>
-      <c r="C85" t="s">
-        <v>197</v>
+      <c r="C85" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="E85" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="F85" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A86" s="6" t="s">
-        <v>199</v>
-      </c>
       <c r="B86" s="6">
         <v>85</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>200</v>
+      <c r="C86" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="E86" t="s">
-        <v>218</v>
+        <v>258</v>
       </c>
       <c r="F86" t="s">
         <v>55</v>
@@ -3391,11 +3821,11 @@
       <c r="B87" s="6">
         <v>86</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>201</v>
+      <c r="C87" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="E87" t="s">
-        <v>219</v>
+        <v>259</v>
       </c>
       <c r="F87" t="s">
         <v>55</v>
@@ -3405,11 +3835,11 @@
       <c r="B88" s="6">
         <v>87</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>202</v>
+      <c r="C88" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="E88" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="F88" t="s">
         <v>55</v>
@@ -3419,11 +3849,11 @@
       <c r="B89" s="6">
         <v>88</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>203</v>
+      <c r="C89" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="E89" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="F89" t="s">
         <v>55</v>
@@ -3433,709 +3863,1520 @@
       <c r="B90" s="6">
         <v>89</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>204</v>
+      <c r="C90" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D90" t="s">
+        <v>375</v>
       </c>
       <c r="E90" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="F90" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A91" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="B91" s="6">
         <v>90</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E91" s="15" t="s">
-        <v>250</v>
+      <c r="C91" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E91" t="s">
+        <v>263</v>
+      </c>
+      <c r="F91" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B92" s="6">
         <v>91</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>232</v>
+      <c r="C92" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="E92" t="s">
-        <v>251</v>
+        <v>264</v>
+      </c>
+      <c r="F92" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B93" s="6">
         <v>92</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>233</v>
+      <c r="C93" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="E93" t="s">
-        <v>252</v>
+        <v>265</v>
+      </c>
+      <c r="F93" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A94" s="6" t="s">
+        <v>266</v>
+      </c>
       <c r="B94" s="6">
         <v>93</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>234</v>
+      <c r="C94" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="E94" t="s">
-        <v>253</v>
+        <v>290</v>
+      </c>
+      <c r="F94" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B95" s="6">
         <v>94</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>235</v>
+      <c r="C95" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="E95" t="s">
-        <v>254</v>
+        <v>291</v>
+      </c>
+      <c r="F95" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B96" s="6">
         <v>95</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>236</v>
+      <c r="C96" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="E96" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+        <v>292</v>
+      </c>
+      <c r="F96" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B97" s="6">
         <v>96</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>237</v>
+      <c r="C97" s="7" t="s">
+        <v>270</v>
       </c>
       <c r="E97" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
+        <v>293</v>
+      </c>
+      <c r="F97" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B98" s="6">
         <v>97</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>238</v>
+      <c r="C98" s="7" t="s">
+        <v>271</v>
       </c>
       <c r="E98" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+        <v>294</v>
+      </c>
+      <c r="F98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B99" s="6">
         <v>98</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>239</v>
+      <c r="C99" s="7" t="s">
+        <v>272</v>
       </c>
       <c r="E99" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
+        <v>295</v>
+      </c>
+      <c r="F99" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B100" s="6">
         <v>99</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>240</v>
+      <c r="C100" s="7" t="s">
+        <v>273</v>
       </c>
       <c r="E100" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
+        <v>297</v>
+      </c>
+      <c r="F100" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B101" s="6">
         <v>100</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>241</v>
+      <c r="C101" s="7" t="s">
+        <v>274</v>
       </c>
       <c r="E101" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
+        <v>296</v>
+      </c>
+      <c r="F101" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B102" s="6">
         <v>101</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>242</v>
+      <c r="C102" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="E102" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
+        <v>298</v>
+      </c>
+      <c r="F102" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B103" s="6">
         <v>102</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>243</v>
+      <c r="C103" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="E103" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
+        <v>299</v>
+      </c>
+      <c r="F103" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B104" s="6">
         <v>103</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>244</v>
+      <c r="C104" s="7" t="s">
+        <v>277</v>
       </c>
       <c r="E104" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
+        <v>300</v>
+      </c>
+      <c r="F104" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B105" s="6">
         <v>104</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>245</v>
+      <c r="C105" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="E105" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
+        <v>301</v>
+      </c>
+      <c r="F105" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B106" s="6">
         <v>105</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>246</v>
+      <c r="C106" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="E106" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
+        <v>302</v>
+      </c>
+      <c r="F106" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B107" s="6">
         <v>106</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>247</v>
+      <c r="C107" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="E107" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
+        <v>303</v>
+      </c>
+      <c r="F107" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B108" s="6">
         <v>107</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>248</v>
+      <c r="C108" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="E108" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
+        <v>304</v>
+      </c>
+      <c r="F108" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B109" s="6">
         <v>108</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>249</v>
+      <c r="C109" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="E109" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A110" s="6" t="s">
-        <v>269</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="F109" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B110" s="6">
         <v>109</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>270</v>
+      <c r="C110" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="E110" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
+        <v>306</v>
+      </c>
+      <c r="F110" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B111" s="6">
         <v>110</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>271</v>
+      <c r="C111" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="E111" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
+        <v>307</v>
+      </c>
+      <c r="F111" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B112" s="6">
         <v>111</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E112" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C112" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="F112" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B113" s="6">
         <v>112</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>273</v>
+      <c r="C113" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="E113" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.4">
+        <v>309</v>
+      </c>
+      <c r="F113" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B114" s="6">
         <v>113</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>274</v>
+      <c r="C114" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="E114" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.4">
+        <v>310</v>
+      </c>
+      <c r="F114" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A115" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="B115" s="6">
         <v>114</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>275</v>
+      <c r="C115" t="s">
+        <v>312</v>
       </c>
       <c r="E115" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.4">
+        <v>337</v>
+      </c>
+      <c r="F115" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B116" s="6">
         <v>115</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>276</v>
+      <c r="C116" t="s">
+        <v>313</v>
       </c>
       <c r="E116" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.4">
+        <v>338</v>
+      </c>
+      <c r="F116" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B117" s="6">
         <v>116</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>277</v>
+      <c r="C117" t="s">
+        <v>314</v>
       </c>
       <c r="E117" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.4">
+        <v>339</v>
+      </c>
+      <c r="F117" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B118" s="6">
         <v>117</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>278</v>
+      <c r="C118" t="s">
+        <v>315</v>
       </c>
       <c r="E118" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.4">
+        <v>340</v>
+      </c>
+      <c r="F118" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B119" s="6">
         <v>118</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>279</v>
+      <c r="C119" t="s">
+        <v>316</v>
       </c>
       <c r="E119" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.4">
+        <v>341</v>
+      </c>
+      <c r="F119" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B120" s="6">
         <v>119</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>280</v>
+      <c r="C120" t="s">
+        <v>317</v>
       </c>
       <c r="E120" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.4">
+        <v>342</v>
+      </c>
+      <c r="F120" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B121" s="6">
         <v>120</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>281</v>
+      <c r="C121" t="s">
+        <v>318</v>
       </c>
       <c r="E121" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.4">
+        <v>343</v>
+      </c>
+      <c r="F121" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B122" s="6">
         <v>121</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>282</v>
+      <c r="C122" t="s">
+        <v>319</v>
       </c>
       <c r="E122" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.4">
+        <v>344</v>
+      </c>
+      <c r="F122" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B123" s="6">
         <v>122</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>283</v>
+      <c r="C123" t="s">
+        <v>320</v>
       </c>
       <c r="E123" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.4">
+        <v>345</v>
+      </c>
+      <c r="F123" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B124" s="6">
         <v>123</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>284</v>
+      <c r="C124" t="s">
+        <v>321</v>
       </c>
       <c r="E124" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.4">
+        <v>346</v>
+      </c>
+      <c r="F124" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B125" s="6">
         <v>124</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>285</v>
+      <c r="C125" t="s">
+        <v>322</v>
       </c>
       <c r="E125" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.4">
+        <v>347</v>
+      </c>
+      <c r="F125" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B126" s="6">
         <v>125</v>
       </c>
-      <c r="C126" s="3" t="s">
-        <v>286</v>
+      <c r="C126" t="s">
+        <v>323</v>
       </c>
       <c r="E126" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.4">
+        <v>348</v>
+      </c>
+      <c r="F126" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B127" s="6">
         <v>126</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>287</v>
+      <c r="C127" t="s">
+        <v>324</v>
       </c>
       <c r="E127" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.4">
+        <v>349</v>
+      </c>
+      <c r="F127" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B128" s="6">
         <v>127</v>
       </c>
-      <c r="C128" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="E128" s="15" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C128" t="s">
+        <v>325</v>
+      </c>
+      <c r="E128" t="s">
+        <v>360</v>
+      </c>
+      <c r="F128" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B129" s="6">
         <v>128</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>289</v>
+      <c r="C129" t="s">
+        <v>326</v>
       </c>
       <c r="E129" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
+        <v>350</v>
+      </c>
+      <c r="F129" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B130" s="6">
         <v>129</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>290</v>
+      <c r="C130" t="s">
+        <v>327</v>
       </c>
       <c r="E130" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A131" s="6" t="s">
-        <v>314</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="F130" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B131" s="6">
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="E131" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
+        <v>361</v>
+      </c>
+      <c r="F131" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B132" s="6">
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="E132" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
+        <v>352</v>
+      </c>
+      <c r="F132" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B133" s="6">
         <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="E133" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
+        <v>353</v>
+      </c>
+      <c r="F133" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B134" s="6">
         <v>133</v>
       </c>
       <c r="C134" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="E134" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
+        <v>354</v>
+      </c>
+      <c r="F134" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B135" s="6">
         <v>134</v>
       </c>
       <c r="C135" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="E135" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
+        <v>355</v>
+      </c>
+      <c r="F135" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B136" s="6">
         <v>135</v>
       </c>
       <c r="C136" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="E136" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
+        <v>356</v>
+      </c>
+      <c r="F136" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B137" s="6">
         <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="E137" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
+        <v>357</v>
+      </c>
+      <c r="F137" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B138" s="6">
         <v>137</v>
       </c>
       <c r="C138" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E138" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
+        <v>358</v>
+      </c>
+      <c r="F138" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B139" s="6">
         <v>138</v>
       </c>
       <c r="C139" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="E139" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
+        <v>359</v>
+      </c>
+      <c r="F139" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A140" s="6" t="s">
+        <v>362</v>
+      </c>
       <c r="B140" s="6">
         <v>139</v>
       </c>
-      <c r="C140" t="s">
-        <v>324</v>
+      <c r="C140" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D140" t="s">
+        <v>364</v>
       </c>
       <c r="E140" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.4">
+        <v>378</v>
+      </c>
+      <c r="F140" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B141" s="6">
         <v>140</v>
       </c>
-      <c r="C141" t="s">
-        <v>325</v>
+      <c r="C141" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D141" t="s">
+        <v>366</v>
       </c>
       <c r="E141" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
+        <v>379</v>
+      </c>
+      <c r="F141" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B142" s="6">
         <v>141</v>
       </c>
-      <c r="C142" t="s">
-        <v>326</v>
-      </c>
-      <c r="E142" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C142" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D142" t="s">
+        <v>368</v>
+      </c>
+      <c r="E142" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="F142" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B143" s="6">
         <v>142</v>
       </c>
-      <c r="C143" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C143" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D143" t="s">
+        <v>370</v>
+      </c>
+      <c r="E143" t="s">
+        <v>381</v>
+      </c>
+      <c r="F143" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B144" s="6">
         <v>143</v>
       </c>
-      <c r="C144" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C144" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D144" t="s">
+        <v>372</v>
+      </c>
+      <c r="E144" t="s">
+        <v>382</v>
+      </c>
+      <c r="F144" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B145" s="6">
         <v>144</v>
       </c>
-      <c r="C145" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C145" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D145" t="s">
+        <v>374</v>
+      </c>
+      <c r="E145" t="s">
+        <v>383</v>
+      </c>
+      <c r="F145" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B146" s="6">
         <v>145</v>
       </c>
-      <c r="C146" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C146" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D146" t="s">
+        <v>377</v>
+      </c>
+      <c r="E146" t="s">
+        <v>384</v>
+      </c>
+      <c r="F146" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A147" s="6" t="s">
+        <v>385</v>
+      </c>
       <c r="B147" s="6">
         <v>146</v>
       </c>
-      <c r="C147" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C147" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="E147" t="s">
+        <v>434</v>
+      </c>
+      <c r="F147" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B148" s="6">
         <v>147</v>
       </c>
-      <c r="C148" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C148" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D148" t="s">
+        <v>389</v>
+      </c>
+      <c r="E148" t="s">
+        <v>435</v>
+      </c>
+      <c r="F148" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B149" s="6">
         <v>148</v>
       </c>
-      <c r="C149" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C149" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="D149" t="s">
+        <v>391</v>
+      </c>
+      <c r="E149" t="s">
+        <v>436</v>
+      </c>
+      <c r="F149" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B150" s="6">
         <v>149</v>
       </c>
-      <c r="C150" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C150" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D150" t="s">
+        <v>393</v>
+      </c>
+      <c r="E150" t="s">
+        <v>437</v>
+      </c>
+      <c r="F150" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B151" s="6">
         <v>150</v>
       </c>
-      <c r="C151" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C151" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="D151" t="s">
+        <v>395</v>
+      </c>
+      <c r="E151" t="s">
+        <v>438</v>
+      </c>
+      <c r="F151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B152" s="6">
         <v>151</v>
       </c>
-      <c r="C152" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C152" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="D152" t="s">
+        <v>397</v>
+      </c>
+      <c r="E152" t="s">
+        <v>439</v>
+      </c>
+      <c r="F152" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B153" s="6">
         <v>152</v>
       </c>
-      <c r="C153" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C153" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D153" t="s">
+        <v>399</v>
+      </c>
+      <c r="E153" t="s">
+        <v>440</v>
+      </c>
+      <c r="F153" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B154" s="6">
         <v>153</v>
       </c>
-      <c r="C154" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C154" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="D154" t="s">
+        <v>401</v>
+      </c>
+      <c r="E154" t="s">
+        <v>441</v>
+      </c>
+      <c r="F154" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B155" s="6">
         <v>154</v>
       </c>
-      <c r="C155" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="C155" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="D155" t="s">
+        <v>403</v>
+      </c>
+      <c r="E155" t="s">
+        <v>442</v>
+      </c>
+      <c r="F155" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B156" s="6">
         <v>155</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="D156" t="s">
+        <v>406</v>
+      </c>
+      <c r="E156" t="s">
+        <v>445</v>
+      </c>
+      <c r="F156" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B157" s="6">
+        <v>156</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D157" t="s">
+        <v>408</v>
+      </c>
+      <c r="E157" t="s">
+        <v>446</v>
+      </c>
+      <c r="F157" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B158" s="6">
+        <v>157</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="D158" t="s">
+        <v>410</v>
+      </c>
+      <c r="E158" t="s">
+        <v>447</v>
+      </c>
+      <c r="F158" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B159" s="6">
+        <v>158</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D159" t="s">
+        <v>412</v>
+      </c>
+      <c r="E159" t="s">
+        <v>448</v>
+      </c>
+      <c r="F159" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B160" s="6">
+        <v>159</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="D160" t="s">
+        <v>414</v>
+      </c>
+      <c r="E160" t="s">
+        <v>449</v>
+      </c>
+      <c r="F160" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B161" s="6">
+        <v>160</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D161" t="s">
+        <v>416</v>
+      </c>
+      <c r="E161" t="s">
+        <v>450</v>
+      </c>
+      <c r="F161" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B162" s="6">
+        <v>161</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D162" t="s">
+        <v>418</v>
+      </c>
+      <c r="E162" t="s">
+        <v>451</v>
+      </c>
+      <c r="F162" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B163" s="6">
+        <v>162</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="D163" t="s">
+        <v>433</v>
+      </c>
+      <c r="E163" t="s">
+        <v>452</v>
+      </c>
+      <c r="F163" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B164" s="6">
+        <v>163</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D164" t="s">
+        <v>420</v>
+      </c>
+      <c r="E164" t="s">
+        <v>453</v>
+      </c>
+      <c r="F164" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B165" s="6">
+        <v>164</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D165" t="s">
+        <v>422</v>
+      </c>
+      <c r="E165" t="s">
+        <v>454</v>
+      </c>
+      <c r="F165" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B166" s="6">
+        <v>165</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="D166" t="s">
+        <v>424</v>
+      </c>
+      <c r="E166" t="s">
+        <v>455</v>
+      </c>
+      <c r="F166" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B167" s="6">
+        <v>166</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="D167" t="s">
+        <v>426</v>
+      </c>
+      <c r="E167" t="s">
+        <v>456</v>
+      </c>
+      <c r="F167" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B168" s="6">
+        <v>167</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="D168" t="s">
+        <v>428</v>
+      </c>
+      <c r="E168" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="F168" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B169" s="6">
+        <v>168</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D169" t="s">
+        <v>430</v>
+      </c>
+      <c r="E169" t="s">
+        <v>458</v>
+      </c>
+      <c r="F169" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B170" s="6">
+        <v>169</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D170" t="s">
+        <v>432</v>
+      </c>
+      <c r="E170" t="s">
+        <v>459</v>
+      </c>
+      <c r="F170" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A171" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B171" s="6">
+        <v>170</v>
+      </c>
+      <c r="C171" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" t="s">
+        <v>14</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F171" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B172" s="6">
+        <v>171</v>
+      </c>
+      <c r="C172" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D172" t="s">
+        <v>13</v>
+      </c>
+      <c r="E172" t="s">
+        <v>38</v>
+      </c>
+      <c r="F172" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B173" s="6">
+        <v>172</v>
+      </c>
+      <c r="C173" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" t="s">
+        <v>41</v>
+      </c>
+      <c r="F173" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B174" s="6">
+        <v>173</v>
+      </c>
+      <c r="C174" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D174" t="s">
+        <v>12</v>
+      </c>
+      <c r="E174" t="s">
+        <v>39</v>
+      </c>
+      <c r="F174" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B175" s="6">
+        <v>174</v>
+      </c>
+      <c r="C175" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D175" t="s">
+        <v>16</v>
+      </c>
+      <c r="E175" t="s">
+        <v>40</v>
+      </c>
+      <c r="F175" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B176" s="6">
+        <v>175</v>
+      </c>
+      <c r="C176" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D176" t="s">
+        <v>18</v>
+      </c>
+      <c r="E176" t="s">
+        <v>42</v>
+      </c>
+      <c r="F176" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B177" s="6">
+        <v>176</v>
+      </c>
+      <c r="C177" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D177" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177" t="s">
+        <v>43</v>
+      </c>
+      <c r="F177" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B178" s="6">
+        <v>177</v>
+      </c>
+      <c r="C178" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D178" t="s">
+        <v>34</v>
+      </c>
+      <c r="E178" t="s">
+        <v>44</v>
+      </c>
+      <c r="F178" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B179" s="6">
+        <v>178</v>
+      </c>
+      <c r="C179" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D179" t="s">
+        <v>33</v>
+      </c>
+      <c r="E179" t="s">
+        <v>45</v>
+      </c>
+      <c r="F179" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B180" s="6">
+        <v>179</v>
+      </c>
+      <c r="C180" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D180" t="s">
+        <v>22</v>
+      </c>
+      <c r="E180" t="s">
+        <v>46</v>
+      </c>
+      <c r="F180" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B181" s="6">
+        <v>180</v>
+      </c>
+      <c r="C181" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D181" t="s">
+        <v>24</v>
+      </c>
+      <c r="E181" t="s">
+        <v>47</v>
+      </c>
+      <c r="F181" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B182" s="6">
+        <v>181</v>
+      </c>
+      <c r="C182" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D182" t="s">
+        <v>26</v>
+      </c>
+      <c r="E182" t="s">
+        <v>48</v>
+      </c>
+      <c r="F182" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="183" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B183" s="6">
+        <v>182</v>
+      </c>
+      <c r="C183" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D183" t="s">
+        <v>28</v>
+      </c>
+      <c r="E183" t="s">
+        <v>49</v>
+      </c>
+      <c r="F183" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B184" s="6">
+        <v>183</v>
+      </c>
+      <c r="C184" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D184" t="s">
+        <v>30</v>
+      </c>
+      <c r="E184" t="s">
+        <v>51</v>
+      </c>
+      <c r="F184" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B185" s="6">
+        <v>184</v>
+      </c>
+      <c r="C185" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" t="s">
+        <v>35</v>
+      </c>
+      <c r="E185" t="s">
+        <v>52</v>
+      </c>
+      <c r="F185" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B186" s="6">
+        <v>185</v>
+      </c>
+      <c r="C186" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D186" t="s">
+        <v>32</v>
+      </c>
+      <c r="E186" t="s">
+        <v>53</v>
+      </c>
+      <c r="F186" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4143,8 +5384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4927,7 +6168,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5129,10 +6370,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5142,18 +6383,18 @@
     <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>467</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5163,131 +6404,143 @@
       <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>464</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>465</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="6">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="6">
         <v>6</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="6">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="6">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="6">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="6">
         <v>12</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="6">
         <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="6">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="6">
         <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5296,6 +6549,46 @@
         <v>16</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
S04P12A401-117 [+] Edit DB recipe 데킬라
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_total.xlsx
+++ b/DB/cocktailDB/cocktailDB_total.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="article" sheetId="2" r:id="rId1"/>
-    <sheet name="article-alcohol" sheetId="4" r:id="rId2"/>
-    <sheet name="alcohol" sheetId="6" r:id="rId3"/>
-    <sheet name="ingredient" sheetId="1" r:id="rId4"/>
-    <sheet name="recipe" sheetId="3" r:id="rId5"/>
+    <sheet name="recipe" sheetId="3" r:id="rId2"/>
+    <sheet name="article-alcohol" sheetId="4" r:id="rId3"/>
+    <sheet name="alcohol" sheetId="6" r:id="rId4"/>
+    <sheet name="ingredient" sheetId="1" r:id="rId5"/>
     <sheet name="cup" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="499">
   <si>
     <t>기저 주류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2030,23 +2030,147 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>넣어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>섞어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>따라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마셔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cocktail_pk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 사워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desert water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acouplecooks.com/wp-content/uploads/2020/04/Tequila-Sour-005.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila sour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila sunrise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데저트워터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칵테일 쉐이커에 얼음을 넣고 30 초 동안 다시 흔듭니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acouplecooks.com/wp-content/uploads/2020/04/Tequila-Sunrise-003.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음료수를 잔에 넣고 라임이나 체리로 가니쉬합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가니쉬로 라임, 체리 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그레나딘 시럽을 음료 중앙에 부으면 바닥에 가라 앉습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일출 그라데이션 효과를 위해 부드럽게 저어주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼음없이 칵테일 셰이커에 재료를 넣고 15 초 동안 흔들어 주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이볼 잔에 얼음을 채웁니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라와 오렌지 주스를 붓고 저어주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가니쉬로 오렌지, 체리 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오렌지 슬라이스와 체리로 가니쉬 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila sunset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://hips.hearstapps.com/del.h-cdn.co/assets/15/36/1441227327-thirsty-thursday-tequila-sunrise.jpg?crop=0.4444444444444444xw:1xh;center,top&amp;resize=980:*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.haveacocktail.com/images/da/7081.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila stone sour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 선셋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라와 레몬 주스를 붓고 저어주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일몰 그라데이션 효과를 위해 부드럽게 저어주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 스톤 사워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온더락 잔에 부어 주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila slammer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/originals/3c/8e/dd/3c8edd5dc88ba624ede5644c6c078c35.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 위에 탄산수를 따라주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔의 주둥이를 냅킨으로 덮고 손바닥으로 감싸 쥐고 테이블에 내려칩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데킬라 토닉</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2054,7 +2178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2108,13 +2232,28 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -2203,12 +2342,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2263,9 +2405,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2543,21 +2692,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="8.796875" style="6"/>
-    <col min="3" max="3" width="27.59765625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="20.3984375" customWidth="1"/>
-    <col min="5" max="5" width="39.5" customWidth="1"/>
+    <col min="1" max="1" width="3" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="8" max="8" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2579,16 +2730,22 @@
       <c r="G1" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H1" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="17" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
+      <c r="C2" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="D2" t="s">
+        <v>465</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>461</v>
@@ -2596,14 +2753,20 @@
       <c r="F2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="17"/>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>464</v>
+      </c>
+      <c r="D3" t="s">
+        <v>467</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>131</v>
@@ -2611,8 +2774,14 @@
       <c r="F3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G3" s="20" t="s">
+        <v>466</v>
+      </c>
+      <c r="H3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="17"/>
       <c r="B4" s="6">
         <v>3</v>
@@ -2620,14 +2789,23 @@
       <c r="C4" t="s">
         <v>76</v>
       </c>
+      <c r="D4" t="s">
+        <v>468</v>
+      </c>
       <c r="E4" s="14" t="s">
         <v>132</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G4" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="H4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="17"/>
       <c r="B5" s="6">
         <v>4</v>
@@ -2635,14 +2813,23 @@
       <c r="C5" t="s">
         <v>77</v>
       </c>
+      <c r="D5" t="s">
+        <v>485</v>
+      </c>
       <c r="E5" s="14" t="s">
         <v>462</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G5" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="H5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="17"/>
       <c r="B6" s="6">
         <v>5</v>
@@ -2650,14 +2837,20 @@
       <c r="C6" t="s">
         <v>78</v>
       </c>
+      <c r="D6" t="s">
+        <v>488</v>
+      </c>
       <c r="E6" s="14" t="s">
         <v>133</v>
       </c>
       <c r="F6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G6" s="20" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="17"/>
       <c r="B7" s="6">
         <v>6</v>
@@ -2665,14 +2858,20 @@
       <c r="C7" t="s">
         <v>79</v>
       </c>
+      <c r="D7" t="s">
+        <v>494</v>
+      </c>
       <c r="E7" s="14" t="s">
         <v>134</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G7" s="20" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="17"/>
       <c r="B8" s="6">
         <v>7</v>
@@ -2687,7 +2886,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="17"/>
       <c r="B9" s="6">
         <v>8</v>
@@ -2702,7 +2901,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="17"/>
       <c r="B10" s="6">
         <v>9</v>
@@ -2717,7 +2916,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="17"/>
       <c r="B11" s="6">
         <v>10</v>
@@ -2732,7 +2931,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
       <c r="B12" s="6">
         <v>11</v>
@@ -2747,7 +2946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
       <c r="B13" s="6">
         <v>12</v>
@@ -2762,7 +2961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="17"/>
       <c r="B14" s="6">
         <v>13</v>
@@ -2777,7 +2976,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="17"/>
       <c r="B15" s="6">
         <v>14</v>
@@ -2792,7 +2991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="17"/>
       <c r="B16" s="6">
         <v>15</v>
@@ -5375,17 +5574,1688 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H185"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.09765625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="3"/>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="3"/>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>476</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>481</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="3"/>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>482</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="3"/>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>478</v>
+      </c>
+      <c r="G7" s="6">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="3"/>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>479</v>
+      </c>
+      <c r="G8" s="6">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="3"/>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>484</v>
+      </c>
+      <c r="G9" s="6">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>489</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G10" s="6">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="3"/>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>490</v>
+      </c>
+      <c r="G11" s="6">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="3"/>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>478</v>
+      </c>
+      <c r="G12" s="6">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="3"/>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>491</v>
+      </c>
+      <c r="G13" s="6">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="3"/>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>484</v>
+      </c>
+      <c r="G14" s="6">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>492</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>480</v>
+      </c>
+      <c r="G15" s="6">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="3"/>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>493</v>
+      </c>
+      <c r="G16" s="6">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>496</v>
+      </c>
+      <c r="G17" s="6">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>497</v>
+      </c>
+      <c r="G18" s="6">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B19" s="6">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>498</v>
+      </c>
+      <c r="G19" s="6">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G20" s="6">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G21" s="6">
+        <v>21</v>
+      </c>
+      <c r="H21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G22" s="6">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G23" s="6">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G24" s="6">
+        <v>24</v>
+      </c>
+      <c r="H24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G25" s="6">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G26" s="6">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G27" s="6">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G28" s="6">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G29" s="6">
+        <v>29</v>
+      </c>
+      <c r="H29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G30" s="6">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G31" s="6">
+        <v>31</v>
+      </c>
+      <c r="H31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="G32" s="6">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G33" s="6">
+        <v>33</v>
+      </c>
+      <c r="H33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G34" s="6">
+        <v>34</v>
+      </c>
+      <c r="H34" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="G35" s="6">
+        <v>35</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="G36" s="6">
+        <v>36</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G37" s="6">
+        <v>37</v>
+      </c>
+      <c r="H37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G38" s="6">
+        <v>38</v>
+      </c>
+      <c r="H38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G39" s="6">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G40" s="6">
+        <v>40</v>
+      </c>
+      <c r="H40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G41" s="6">
+        <v>41</v>
+      </c>
+      <c r="H41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G42" s="6">
+        <v>42</v>
+      </c>
+      <c r="H42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G43" s="6">
+        <v>43</v>
+      </c>
+      <c r="H43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G44" s="6">
+        <v>44</v>
+      </c>
+      <c r="H44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G45" s="6">
+        <v>45</v>
+      </c>
+      <c r="H45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G46" s="6">
+        <v>46</v>
+      </c>
+      <c r="H46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G47" s="6">
+        <v>47</v>
+      </c>
+      <c r="H47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G48" s="6">
+        <v>48</v>
+      </c>
+      <c r="H48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G49" s="6">
+        <v>49</v>
+      </c>
+      <c r="H49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G50" s="6">
+        <v>50</v>
+      </c>
+      <c r="H50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G51" s="6">
+        <v>51</v>
+      </c>
+      <c r="H51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G52" s="6">
+        <v>52</v>
+      </c>
+      <c r="H52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G53" s="6">
+        <v>53</v>
+      </c>
+      <c r="H53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G54" s="6">
+        <v>54</v>
+      </c>
+      <c r="H54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G55" s="6">
+        <v>55</v>
+      </c>
+      <c r="H55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G56" s="6">
+        <v>56</v>
+      </c>
+      <c r="H56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G57" s="6">
+        <v>57</v>
+      </c>
+      <c r="H57" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G58" s="6">
+        <v>58</v>
+      </c>
+      <c r="H58" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G59" s="6">
+        <v>59</v>
+      </c>
+      <c r="H59" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="60" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G60" s="6">
+        <v>60</v>
+      </c>
+      <c r="H60" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G61" s="6">
+        <v>61</v>
+      </c>
+      <c r="H61" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G62" s="6">
+        <v>62</v>
+      </c>
+      <c r="H62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G63" s="6">
+        <v>63</v>
+      </c>
+      <c r="H63" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G64" s="6">
+        <v>64</v>
+      </c>
+      <c r="H64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G65" s="6">
+        <v>65</v>
+      </c>
+      <c r="H65" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G66" s="6">
+        <v>66</v>
+      </c>
+      <c r="H66" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G67" s="6">
+        <v>67</v>
+      </c>
+      <c r="H67" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="68" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G68" s="6">
+        <v>68</v>
+      </c>
+      <c r="H68" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G69" s="6">
+        <v>69</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G70" s="6">
+        <v>70</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="71" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G71" s="6">
+        <v>71</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G72" s="6">
+        <v>72</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G73" s="6">
+        <v>73</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G74" s="6">
+        <v>74</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G75" s="6">
+        <v>75</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G76" s="6">
+        <v>76</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="77" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G77" s="6">
+        <v>77</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G78" s="6">
+        <v>78</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G79" s="6">
+        <v>79</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="80" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G80" s="6">
+        <v>80</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G81" s="6">
+        <v>81</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G82" s="6">
+        <v>82</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G83" s="6">
+        <v>83</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G84" s="6">
+        <v>84</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G85" s="6">
+        <v>85</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="86" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G86" s="6">
+        <v>86</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="87" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G87" s="6">
+        <v>87</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="88" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G88" s="6">
+        <v>88</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="89" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G89" s="6">
+        <v>89</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G90" s="6">
+        <v>90</v>
+      </c>
+      <c r="H90" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G91" s="6">
+        <v>91</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G92" s="6">
+        <v>92</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G93" s="6">
+        <v>93</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="94" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G94" s="6">
+        <v>94</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="95" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G95" s="6">
+        <v>95</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G96" s="6">
+        <v>96</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G97" s="6">
+        <v>97</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="98" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G98" s="6">
+        <v>98</v>
+      </c>
+      <c r="H98" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="99" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G99" s="6">
+        <v>99</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="100" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G100" s="6">
+        <v>100</v>
+      </c>
+      <c r="H100" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="101" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G101" s="6">
+        <v>101</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="102" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G102" s="6">
+        <v>102</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G103" s="6">
+        <v>103</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G104" s="6">
+        <v>104</v>
+      </c>
+      <c r="H104" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="105" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G105" s="6">
+        <v>105</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="106" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G106" s="6">
+        <v>106</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G107" s="6">
+        <v>107</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="108" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G108" s="6">
+        <v>108</v>
+      </c>
+      <c r="H108" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="109" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G109" s="6">
+        <v>109</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G110" s="6">
+        <v>110</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="111" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G111" s="6">
+        <v>111</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="112" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G112" s="6">
+        <v>112</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G113" s="6">
+        <v>113</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="114" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G114" s="6">
+        <v>114</v>
+      </c>
+      <c r="H114" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="115" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G115" s="6">
+        <v>115</v>
+      </c>
+      <c r="H115" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="116" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G116" s="6">
+        <v>116</v>
+      </c>
+      <c r="H116" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="117" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G117" s="6">
+        <v>117</v>
+      </c>
+      <c r="H117" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="118" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G118" s="6">
+        <v>118</v>
+      </c>
+      <c r="H118" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="119" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G119" s="6">
+        <v>119</v>
+      </c>
+      <c r="H119" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="120" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G120" s="6">
+        <v>120</v>
+      </c>
+      <c r="H120" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="121" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G121" s="6">
+        <v>121</v>
+      </c>
+      <c r="H121" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="122" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G122" s="6">
+        <v>122</v>
+      </c>
+      <c r="H122" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="123" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G123" s="6">
+        <v>123</v>
+      </c>
+      <c r="H123" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="124" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G124" s="6">
+        <v>124</v>
+      </c>
+      <c r="H124" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="125" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G125" s="6">
+        <v>125</v>
+      </c>
+      <c r="H125" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="126" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G126" s="6">
+        <v>126</v>
+      </c>
+      <c r="H126" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="127" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G127" s="6">
+        <v>127</v>
+      </c>
+      <c r="H127" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="128" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G128" s="6">
+        <v>128</v>
+      </c>
+      <c r="H128" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="129" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G129" s="6">
+        <v>129</v>
+      </c>
+      <c r="H129" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="130" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G130" s="6">
+        <v>130</v>
+      </c>
+      <c r="H130" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="131" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G131" s="6">
+        <v>131</v>
+      </c>
+      <c r="H131" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="132" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G132" s="6">
+        <v>132</v>
+      </c>
+      <c r="H132" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="133" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G133" s="6">
+        <v>133</v>
+      </c>
+      <c r="H133" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="134" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G134" s="6">
+        <v>134</v>
+      </c>
+      <c r="H134" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G135" s="6">
+        <v>135</v>
+      </c>
+      <c r="H135" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="136" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G136" s="6">
+        <v>136</v>
+      </c>
+      <c r="H136" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="137" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G137" s="6">
+        <v>137</v>
+      </c>
+      <c r="H137" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="138" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G138" s="6">
+        <v>138</v>
+      </c>
+      <c r="H138" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="139" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G139" s="6">
+        <v>139</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="140" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G140" s="6">
+        <v>140</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="141" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G141" s="6">
+        <v>141</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="142" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G142" s="6">
+        <v>142</v>
+      </c>
+      <c r="H142" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="143" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G143" s="6">
+        <v>143</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="144" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G144" s="6">
+        <v>144</v>
+      </c>
+      <c r="H144" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="145" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G145" s="6">
+        <v>145</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="146" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G146" s="6">
+        <v>146</v>
+      </c>
+      <c r="H146" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="147" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G147" s="6">
+        <v>147</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="148" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G148" s="6">
+        <v>148</v>
+      </c>
+      <c r="H148" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="149" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G149" s="6">
+        <v>149</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="150" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G150" s="6">
+        <v>150</v>
+      </c>
+      <c r="H150" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="151" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G151" s="6">
+        <v>151</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="152" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G152" s="6">
+        <v>152</v>
+      </c>
+      <c r="H152" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="153" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G153" s="6">
+        <v>153</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="154" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G154" s="6">
+        <v>154</v>
+      </c>
+      <c r="H154" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="155" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G155" s="6">
+        <v>155</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="156" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G156" s="6">
+        <v>156</v>
+      </c>
+      <c r="H156" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="157" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G157" s="6">
+        <v>157</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="158" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G158" s="6">
+        <v>158</v>
+      </c>
+      <c r="H158" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="159" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G159" s="6">
+        <v>159</v>
+      </c>
+      <c r="H159" s="7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="160" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G160" s="6">
+        <v>160</v>
+      </c>
+      <c r="H160" s="7" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="161" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G161" s="6">
+        <v>161</v>
+      </c>
+      <c r="H161" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="162" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G162" s="6">
+        <v>162</v>
+      </c>
+      <c r="H162" s="7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="163" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G163" s="6">
+        <v>163</v>
+      </c>
+      <c r="H163" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="164" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G164" s="6">
+        <v>164</v>
+      </c>
+      <c r="H164" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="165" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G165" s="6">
+        <v>165</v>
+      </c>
+      <c r="H165" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="166" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G166" s="6">
+        <v>166</v>
+      </c>
+      <c r="H166" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="167" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G167" s="6">
+        <v>167</v>
+      </c>
+      <c r="H167" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="168" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G168" s="6">
+        <v>168</v>
+      </c>
+      <c r="H168" s="7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="169" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G169" s="6">
+        <v>169</v>
+      </c>
+      <c r="H169" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="170" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G170" s="6">
+        <v>170</v>
+      </c>
+      <c r="H170" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G171" s="6">
+        <v>171</v>
+      </c>
+      <c r="H171" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="7:8" x14ac:dyDescent="0.4">
+      <c r="G172" s="6">
+        <v>172</v>
+      </c>
+      <c r="H172" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G173" s="6">
+        <v>173</v>
+      </c>
+      <c r="H173" s="19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="174" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G174" s="6">
+        <v>174</v>
+      </c>
+      <c r="H174" s="19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="175" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G175" s="6">
+        <v>175</v>
+      </c>
+      <c r="H175" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="176" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G176" s="6">
+        <v>176</v>
+      </c>
+      <c r="H176" s="19" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="177" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G177" s="6">
+        <v>177</v>
+      </c>
+      <c r="H177" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G178" s="6">
+        <v>178</v>
+      </c>
+      <c r="H178" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G179" s="6">
+        <v>179</v>
+      </c>
+      <c r="H179" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="180" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G180" s="6">
+        <v>180</v>
+      </c>
+      <c r="H180" s="19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="181" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G181" s="6">
+        <v>181</v>
+      </c>
+      <c r="H181" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="182" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G182" s="6">
+        <v>182</v>
+      </c>
+      <c r="H182" s="19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="183" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G183" s="6">
+        <v>183</v>
+      </c>
+      <c r="H183" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="184" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G184" s="6">
+        <v>184</v>
+      </c>
+      <c r="H184" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G185" s="6">
+        <v>185</v>
+      </c>
+      <c r="H185" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6163,7 +8033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -6191,7 +8061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -6361,162 +8231,6 @@
       <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.69921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>464</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>465</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="3"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="3"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
S04P12A401-112 [+]Add 데이터 서치 & 정리 - alcohol
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_total.xlsx
+++ b/DB/cocktailDB/cocktailDB_total.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\s04p12a401\DB\cocktailDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\gitlab\s04p12a401\DB\cocktailDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="article" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="627">
   <si>
     <t>기저 주류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2171,6 +2171,500 @@
   </si>
   <si>
     <t>데킬라 토닉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아무종류의 데킬라나 상관없다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호세쿠엘보 에스페샬 골드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jose Cuervo Especial Gold Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_cue1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51퍼센트의 푸른 용설란 수액과 49퍼센트의 기타 용설란 수액을 재료로 한다. 밝은 황금색의 빛깔을 보여 숙성된 테킬라라 생각하기 쉽지만 사실 이 색깔은 캐러멜 등의 첨가물에 의한 것이다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호세쿠엘보 트라디시오날 레포사도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jose Cuervo Tradicional Reposado Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_cue5.jpg</t>
+  </si>
+  <si>
+    <t>맑고 투명한 금색으로 다른 첨가물 없이 100% 블루 아가베 수액만을 사용하며 최소 2개월 동안 오크통에서 숙성을 거쳐 제조된다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패트론 실버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patron Silver Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_pat1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짧은 숙성기간을 거쳐 부드럽고 깔끔한 맛을 낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패트론 아녜호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patron Anejo Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_pat3.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1년간 숙성하여 진한 풍미를 내는 밝은 금색이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패트론 레포사도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patron Reposado Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_pat2.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패트론 실버와 패트론 아녜호를 잘 혼합하여 6개월 정도 숙성한 술이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈홀리오 블랑코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Julio Blanco Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_don1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깨끗하고 깔끔한 맛으로 데킬라 칵테일에 잘어울린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈훌리오 레포사도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Julio Reposado Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_don3.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감귤향으로 오크통에 8개월 숙성을 거친다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈홀리오 아네호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Julio Anejo Tequila</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/teqla_don2.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카라멜/감귤향으로 위스키가 숙성된 오크통에서 18개월을 숙성시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탱커레이 런던드라이 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanqueray London Dry Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/gin_tan1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>꽃 향기가 나며 산뜻하고 드라이합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탱커레이 No.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanqueray No.10 Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/gin_tan5.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감귤/자몽향으로 마티니에 어울립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핸드릭스 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hendrick's Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/gin_hen15.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11가지 천연허브 원료와 불가리아산 장미 꽃잎, 네덜란드산 오이에서 추출한 오일을 중류과정에서 자연스럽게 스며들게한 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>봄베이 사파이어 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bombay Sapphire Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/gin_bom2.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허브, 약초향으로 토닉과 잘어울립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비피이터 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beefeater Dry Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/gin_bee19.jpg</t>
+  </si>
+  <si>
+    <t>영국 런던의 런던탑을 지키는 요먼 경비대의 별명에서 따온 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고든스 런던 드라이 진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon's London Dry Gin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.gordonsgin.com/media/837953/homepage-export-single-bottle.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영국에서 생산되는 오래된 진으로, 라벨의 동물인 멧돼지는 고든 가문의 상징입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팜페로 블랑코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pampero Blanco Rum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_pam4.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6개월간 숙성을 거치고 모히또 스타일의 칵테일이 어울린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자카파 23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ron Zacapa Centenario Sistema Solera 23 Rum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_ron1.jpg</t>
+  </si>
+  <si>
+    <t>높은 고도에서 숙성하고 6~23년 숙성된 ㄹ머을 블렌딩 합니다. 그 자체를 즐기는것이 좋은 술입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐리비안 럼으로 향신료와 천연재료에서 나오는 향이 훌륭합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캡틴 모건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Captain Morgan Spiced Gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_cap2.jpg</t>
+  </si>
+  <si>
+    <t>플랜테이션 오리지널 다크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plantation Original Dark Rum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_pla29.jpg</t>
+  </si>
+  <si>
+    <t>트로피컬한 칵테일 베이스로 추천합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디플로마티코 익스클루시바</t>
+  </si>
+  <si>
+    <t>Diplomatico Reserva Exclusiva Rum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_dip1.jpg</t>
+  </si>
+  <si>
+    <t>니트 또는 온더락스타일로 그냥 먹거나 올드패션드로 만들어 먹는 것을 추천합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/rum_bac92.jpg</t>
+  </si>
+  <si>
+    <t>바카디 슈페리얼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bacardi Superior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화이트럼으로 모히또를 만들어 마시는 것을 추천합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카차카 51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cachaca 51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브라질 국민주로, 카이피리냐 칵테일 베이스로 잘 알려져있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://wine1865.co.kr/upload/p_image/b/P0714-677.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보드카</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ketel One Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>케텔 원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_ket1.jpg</t>
+  </si>
+  <si>
+    <t>온더락 스타일로 얼음과 라임 한조각을 넣어마신다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스미노프 No.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Smirnoff Red Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_smi3.jpg</t>
+  </si>
+  <si>
+    <t>모스코뮬(moscow mule) 칵테일을 주로 만들어 먹는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스미노프 블랙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_smi14.jpg</t>
+  </si>
+  <si>
+    <t>보드카 토닉 스타일로 먹는 것을 추천한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Smirnoff Black Label Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시로크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_cir2.jpg</t>
+  </si>
+  <si>
+    <t>Ciroc Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레몬 혹은 라임향이 난다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앱솔루트 오리지날</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Absolut Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_abs1.jpg</t>
+  </si>
+  <si>
+    <t>크렌베리 주스나 다른 주스에 섞어서 마시는 걸 추천합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_gre14.jpg</t>
+  </si>
+  <si>
+    <t>그레이 구스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grey Goose Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깔끔한 맛, 부드러운 목 넘김이 특징이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벨베디어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잡맛이 없고 깔끔한 것이 특징으로 혀 끝에서 좀 더 순하며 부드러운 맛을 내고 키스 오브 파이어에 잘어울립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_bel50.jpg</t>
+  </si>
+  <si>
+    <t>Belvedere Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스톨리치나야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stolichnaya Red Vodka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/vodka_sto5.jpg</t>
+  </si>
+  <si>
+    <t>밀과 호밀이 원재료인 러시아산 보드카의 대명사이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브랜디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brandy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hennessy VS Cognac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤네시 VSOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/cognc_hen6.jpg</t>
+  </si>
+  <si>
+    <t>100여가지 이상 혼합하여 독특한 맛과 향을 창조하여 깊으면서도 잘 조화된 맛과 안정적이며 온화한 향으로 인정받는다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2350,7 +2844,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2409,6 +2903,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3287,7 +3784,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B36" s="6">
         <v>35</v>
       </c>
@@ -5590,7 +6087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -8035,15 +8532,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8054,10 +8551,866 @@
         <v>2</v>
       </c>
       <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>499</v>
+      </c>
+      <c r="E3" t="s">
+        <v>501</v>
+      </c>
+      <c r="F3" t="s">
+        <v>502</v>
+      </c>
+      <c r="G3">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>503</v>
+      </c>
+      <c r="I3" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>499</v>
+      </c>
+      <c r="E4" t="s">
+        <v>505</v>
+      </c>
+      <c r="F4" t="s">
+        <v>506</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>507</v>
+      </c>
+      <c r="I4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>499</v>
+      </c>
+      <c r="E5" t="s">
+        <v>509</v>
+      </c>
+      <c r="F5" t="s">
+        <v>510</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>511</v>
+      </c>
+      <c r="I5" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>499</v>
+      </c>
+      <c r="E6" t="s">
+        <v>513</v>
+      </c>
+      <c r="F6" t="s">
+        <v>514</v>
+      </c>
+      <c r="G6">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>515</v>
+      </c>
+      <c r="I6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>499</v>
+      </c>
+      <c r="E7" t="s">
+        <v>517</v>
+      </c>
+      <c r="F7" t="s">
+        <v>518</v>
+      </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>519</v>
+      </c>
+      <c r="I7" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>499</v>
+      </c>
+      <c r="E8" t="s">
+        <v>521</v>
+      </c>
+      <c r="F8" t="s">
+        <v>522</v>
+      </c>
+      <c r="G8">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>523</v>
+      </c>
+      <c r="I8" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E9" t="s">
+        <v>525</v>
+      </c>
+      <c r="F9" t="s">
+        <v>526</v>
+      </c>
+      <c r="G9">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>527</v>
+      </c>
+      <c r="I9" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>499</v>
+      </c>
+      <c r="E10" t="s">
+        <v>529</v>
+      </c>
+      <c r="F10" t="s">
+        <v>530</v>
+      </c>
+      <c r="G10">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>531</v>
+      </c>
+      <c r="I10" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D11" t="s">
+        <v>533</v>
+      </c>
+      <c r="E11" t="s">
+        <v>534</v>
+      </c>
+      <c r="F11" t="s">
+        <v>535</v>
+      </c>
+      <c r="G11">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>536</v>
+      </c>
+      <c r="I11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" t="s">
+        <v>533</v>
+      </c>
+      <c r="E12" t="s">
+        <v>538</v>
+      </c>
+      <c r="F12" t="s">
+        <v>539</v>
+      </c>
+      <c r="G12">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>540</v>
+      </c>
+      <c r="I12" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" t="s">
+        <v>533</v>
+      </c>
+      <c r="E13" t="s">
+        <v>542</v>
+      </c>
+      <c r="F13" t="s">
+        <v>543</v>
+      </c>
+      <c r="G13">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>544</v>
+      </c>
+      <c r="I13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
+        <v>533</v>
+      </c>
+      <c r="E14" t="s">
+        <v>546</v>
+      </c>
+      <c r="F14" t="s">
+        <v>547</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>548</v>
+      </c>
+      <c r="I14" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>533</v>
+      </c>
+      <c r="E15" t="s">
+        <v>550</v>
+      </c>
+      <c r="F15" t="s">
+        <v>551</v>
+      </c>
+      <c r="G15">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>552</v>
+      </c>
+      <c r="I15" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" t="s">
+        <v>533</v>
+      </c>
+      <c r="E16" t="s">
+        <v>554</v>
+      </c>
+      <c r="F16" t="s">
+        <v>555</v>
+      </c>
+      <c r="G16">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
+        <v>556</v>
+      </c>
+      <c r="I16" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E17" t="s">
+        <v>559</v>
+      </c>
+      <c r="F17" t="s">
+        <v>560</v>
+      </c>
+      <c r="G17">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>561</v>
+      </c>
+      <c r="I17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>558</v>
+      </c>
+      <c r="E18" t="s">
+        <v>563</v>
+      </c>
+      <c r="F18" t="s">
+        <v>564</v>
+      </c>
+      <c r="G18">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>565</v>
+      </c>
+      <c r="I18" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>558</v>
+      </c>
+      <c r="E19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F19" t="s">
+        <v>569</v>
+      </c>
+      <c r="G19">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
+        <v>570</v>
+      </c>
+      <c r="I19" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>558</v>
+      </c>
+      <c r="E20" t="s">
+        <v>571</v>
+      </c>
+      <c r="F20" t="s">
+        <v>572</v>
+      </c>
+      <c r="G20">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s">
+        <v>573</v>
+      </c>
+      <c r="I20" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>558</v>
+      </c>
+      <c r="E21" t="s">
+        <v>575</v>
+      </c>
+      <c r="F21" t="s">
+        <v>576</v>
+      </c>
+      <c r="G21">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>577</v>
+      </c>
+      <c r="I21" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>558</v>
+      </c>
+      <c r="E22" t="s">
+        <v>580</v>
+      </c>
+      <c r="F22" t="s">
+        <v>581</v>
+      </c>
+      <c r="G22">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
+        <v>579</v>
+      </c>
+      <c r="I22" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>558</v>
+      </c>
+      <c r="E23" t="s">
+        <v>583</v>
+      </c>
+      <c r="F23" t="s">
+        <v>584</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>586</v>
+      </c>
+      <c r="I23" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>587</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D24" t="s">
+        <v>588</v>
+      </c>
+      <c r="E24" t="s">
+        <v>590</v>
+      </c>
+      <c r="F24" t="s">
+        <v>589</v>
+      </c>
+      <c r="G24">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
+        <v>591</v>
+      </c>
+      <c r="I24" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D25" t="s">
+        <v>588</v>
+      </c>
+      <c r="E25" t="s">
+        <v>593</v>
+      </c>
+      <c r="F25" t="s">
+        <v>594</v>
+      </c>
+      <c r="G25">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s">
+        <v>595</v>
+      </c>
+      <c r="I25" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D26" t="s">
+        <v>588</v>
+      </c>
+      <c r="E26" t="s">
+        <v>597</v>
+      </c>
+      <c r="F26" t="s">
+        <v>600</v>
+      </c>
+      <c r="G26">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>598</v>
+      </c>
+      <c r="I26" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D27" t="s">
+        <v>588</v>
+      </c>
+      <c r="E27" t="s">
+        <v>601</v>
+      </c>
+      <c r="F27" t="s">
+        <v>603</v>
+      </c>
+      <c r="G27">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>602</v>
+      </c>
+      <c r="I27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D28" t="s">
+        <v>588</v>
+      </c>
+      <c r="E28" t="s">
+        <v>605</v>
+      </c>
+      <c r="F28" t="s">
+        <v>606</v>
+      </c>
+      <c r="G28">
+        <v>40</v>
+      </c>
+      <c r="H28" t="s">
+        <v>607</v>
+      </c>
+      <c r="I28" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D29" t="s">
+        <v>588</v>
+      </c>
+      <c r="E29" t="s">
+        <v>610</v>
+      </c>
+      <c r="F29" t="s">
+        <v>611</v>
+      </c>
+      <c r="G29">
+        <v>40</v>
+      </c>
+      <c r="H29" t="s">
+        <v>609</v>
+      </c>
+      <c r="I29" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D30" t="s">
+        <v>588</v>
+      </c>
+      <c r="E30" t="s">
+        <v>613</v>
+      </c>
+      <c r="F30" t="s">
+        <v>616</v>
+      </c>
+      <c r="G30">
+        <v>40</v>
+      </c>
+      <c r="H30" t="s">
+        <v>615</v>
+      </c>
+      <c r="I30" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D31" t="s">
+        <v>588</v>
+      </c>
+      <c r="E31" t="s">
+        <v>617</v>
+      </c>
+      <c r="F31" t="s">
+        <v>618</v>
+      </c>
+      <c r="G31">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s">
+        <v>619</v>
+      </c>
+      <c r="I31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>621</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="D32" t="s">
+        <v>622</v>
+      </c>
+      <c r="E32" t="s">
+        <v>624</v>
+      </c>
+      <c r="F32" t="s">
+        <v>623</v>
+      </c>
+      <c r="G32">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>625</v>
+      </c>
+      <c r="I32" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="D33" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="D34" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
S04P12A401-113 [+] Edit DB recipe 관계형 테이블 정리
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_total.xlsx
+++ b/DB/cocktailDB/cocktailDB_total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" tabRatio="756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" tabRatio="756" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="article" sheetId="9" r:id="rId1"/>
@@ -4422,7 +4422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -7603,7 +7603,7 @@
     <hyperlink ref="G14" r:id="rId12"/>
     <hyperlink ref="G15" r:id="rId13"/>
     <hyperlink ref="G16" r:id="rId14"/>
-    <hyperlink ref="G18"/>
+    <hyperlink ref="G18" display="https://www.liquor.com/thmb/sV0rYbLFAcGvdm4d4M8KGDRwJUE=/720x720/filters:no_upscale():max_bytes(150000):strip_icc()/__opt__aboutcom__coeus__resources__content_migration__liquor__2016__04__20130641__10-Essential-Cocktails-for-Cinco-de-Mayo-the-firecracker-"/>
     <hyperlink ref="G19" r:id="rId15"/>
     <hyperlink ref="G20" r:id="rId16"/>
     <hyperlink ref="G21" r:id="rId17"/>
@@ -7624,7 +7624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -8206,7 +8206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
@@ -10053,7 +10053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
@@ -13095,10 +13095,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -13107,7 +13107,7 @@
     <col min="8" max="8" width="14.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13119,7 +13119,7 @@
       </c>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -13147,8 +13147,12 @@
       <c r="I2" s="13" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J2" t="str">
+        <f>"INSERT INTO alcohol VALUES('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"')"</f>
+        <v>INSERT INTO alcohol VALUES('1','데킬라','Tequila')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>2</v>
       </c>
@@ -13174,7 +13178,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>3</v>
       </c>
@@ -13200,7 +13204,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>4</v>
       </c>
@@ -13226,7 +13230,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>5</v>
       </c>
@@ -13252,7 +13256,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>6</v>
       </c>
@@ -13278,7 +13282,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>7</v>
       </c>
@@ -13304,7 +13308,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>8</v>
       </c>
@@ -13330,7 +13334,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>9</v>
       </c>
@@ -13356,7 +13360,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>273</v>
       </c>
@@ -13385,7 +13389,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>11</v>
       </c>
@@ -13411,7 +13415,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>12</v>
       </c>
@@ -13437,7 +13441,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>13</v>
       </c>
@@ -13463,7 +13467,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>14</v>
       </c>
@@ -13489,7 +13493,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
tag test table 생성
</commit_message>
<xml_diff>
--- a/DB/cocktailDB/cocktailDB_total.xlsx
+++ b/DB/cocktailDB/cocktailDB_total.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" tabRatio="756" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19092" windowHeight="9996" tabRatio="756" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="article" sheetId="9" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="article-ingredient" sheetId="8" r:id="rId5"/>
     <sheet name="ingredient" sheetId="1" r:id="rId6"/>
     <sheet name="alcohol" sheetId="6" r:id="rId7"/>
+    <sheet name="tag" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">article!$C$1:$C$92</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="989">
   <si>
     <t>기저 주류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3887,6 +3888,18 @@
   </si>
   <si>
     <t>https://dimg.donga.com/wps/NEWS/IMAGE/2013/11/20/59008900.4.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content_kor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content_eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>White rum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -13097,8 +13110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -13660,7 +13673,7 @@
         <v>775</v>
       </c>
       <c r="D22" t="s">
-        <v>507</v>
+        <v>988</v>
       </c>
       <c r="E22" t="s">
         <v>529</v>
@@ -14309,4 +14322,184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>987</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"INSERT INTO alcohol VALUES('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"');"</f>
+        <v>INSERT INTO alcohol VALUES('1','데킬라','Tequila','1');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H9" si="0">"INSERT INTO alcohol VALUES('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"');"</f>
+        <v>INSERT INTO alcohol VALUES('2','진','Gin','1');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>774</v>
+      </c>
+      <c r="D4" t="s">
+        <v>988</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('3','화이트 럼','White rum','1');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>507</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('4','럼','Rum','1');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" t="s">
+        <v>537</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('5','보드카','Vodka','1');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>571</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('6','브랜디','Brandy','1');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D8" t="s">
+        <v>727</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('7','리큐르','Liqueur','1');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>883</v>
+      </c>
+      <c r="D9" t="s">
+        <v>886</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO alcohol VALUES('8','버번 위스키','Bourbon whiskey','1');</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>